<commit_message>
Officially Launched Group 1
</commit_message>
<xml_diff>
--- a/Worker List.xlsx
+++ b/Worker List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://simcona-my.sharepoint.com/personal/jxiong_simcona_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_F25DC773A252ABDACC1048AB49DF5EEE5ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E88D2745-8464-4C43-8C32-173585D4FB43}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="11_F25DC773A252ABDACC1048AB49DF5EEE5ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CDA39D1-25E0-45CD-8A25-6D6A075F6FDE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Korey Sugar</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Daisy Moreau</t>
+  </si>
+  <si>
+    <t>ZyAsia Holmes</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -201,15 +204,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,15 +650,18 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17">
         <v>1166</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -649,7 +669,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -657,7 +677,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -665,7 +685,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -673,7 +693,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -681,7 +701,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -689,7 +709,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -697,7 +717,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -705,7 +725,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -713,7 +733,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -721,7 +741,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -729,7 +749,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -737,7 +757,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -745,7 +765,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -753,7 +773,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -776,9 +796,6 @@
       <c r="B34">
         <v>1165</v>
       </c>
-      <c r="C34" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -787,9 +804,6 @@
       <c r="B35">
         <v>1186</v>
       </c>
-      <c r="C35" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -799,6 +813,17 @@
         <v>1151</v>
       </c>
       <c r="C36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37">
+        <v>1185</v>
+      </c>
+      <c r="C37" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Name - TJ
</commit_message>
<xml_diff>
--- a/Worker List.xlsx
+++ b/Worker List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://simcona.sharepoint.com/panel/operations/Data Collection/Scanning Data Processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jxiong\GitCode\TimeData_Processing\TimeData_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{74978578-FC59-4ADD-B0C6-9D2274DDCC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F9B74D3-3913-4691-8C1A-104044213903}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF7F675-81BA-4AC5-881D-8D279C9710EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3240" yWindow="4785" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38745" yWindow="645" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$A$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$A$51</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Name</t>
   </si>
@@ -62,9 +62,6 @@
     <t>N521D5060024</t>
   </si>
   <si>
-    <t>Amit Mallik</t>
-  </si>
-  <si>
     <t>8166BF3C</t>
   </si>
   <si>
@@ -176,193 +173,190 @@
     <t>Jeremy Peden-Dorsey</t>
   </si>
   <si>
+    <t>Joshua Ladd</t>
+  </si>
+  <si>
+    <t>CB46D992</t>
+  </si>
+  <si>
+    <t>N445D50044</t>
+  </si>
+  <si>
+    <t>Justin Blake</t>
+  </si>
+  <si>
+    <t>Justin Sampel</t>
+  </si>
+  <si>
+    <t>Korey Sugar</t>
+  </si>
+  <si>
+    <t>Maria Raquel Pum</t>
+  </si>
+  <si>
+    <t>11D14592</t>
+  </si>
+  <si>
+    <t>N445D50019</t>
+  </si>
+  <si>
+    <t>Mark Zhukov</t>
+  </si>
+  <si>
+    <t>Michael Maksymciw</t>
+  </si>
+  <si>
+    <t>D4C6CF96</t>
+  </si>
+  <si>
+    <t>N515D5060010</t>
+  </si>
+  <si>
+    <t>Michael Tucciarello</t>
+  </si>
+  <si>
+    <t>F72F821E</t>
+  </si>
+  <si>
+    <t>Oleksandr Pogorilov</t>
+  </si>
+  <si>
+    <t>B455EFD2</t>
+  </si>
+  <si>
+    <t>Rashard Moore</t>
+  </si>
+  <si>
+    <t>Reginald Tucker</t>
+  </si>
+  <si>
+    <t>Roedell Williams,</t>
+  </si>
+  <si>
+    <t>0489D091</t>
+  </si>
+  <si>
+    <t>Saad Shamsaldeen</t>
+  </si>
+  <si>
+    <t>Sayed Hossiny</t>
+  </si>
+  <si>
+    <t>BCAFEC01</t>
+  </si>
+  <si>
+    <t>N521D5060027</t>
+  </si>
+  <si>
+    <t>Shondrell Rutley</t>
+  </si>
+  <si>
+    <t>FA02F7A3</t>
+  </si>
+  <si>
+    <t>Steven Dessie</t>
+  </si>
+  <si>
+    <t>Zy'Asia Holmes</t>
+  </si>
+  <si>
+    <t>A46E6932</t>
+  </si>
+  <si>
+    <t>N521D5060009</t>
+  </si>
+  <si>
+    <t>N521D5060032</t>
+  </si>
+  <si>
+    <t>N521D5060020</t>
+  </si>
+  <si>
+    <t>N521D5060015</t>
+  </si>
+  <si>
+    <t>N445D50036</t>
+  </si>
+  <si>
+    <t>N521D5060023</t>
+  </si>
+  <si>
+    <t>N521D5060012</t>
+  </si>
+  <si>
+    <t>EC44ACBC</t>
+  </si>
+  <si>
+    <t>N521D5060026</t>
+  </si>
+  <si>
+    <t>3A5DB840</t>
+  </si>
+  <si>
+    <t>N521D5060006</t>
+  </si>
+  <si>
+    <t>52FBA5FF</t>
+  </si>
+  <si>
+    <t>7A21E43A</t>
+  </si>
+  <si>
+    <t>N521D5060004</t>
+  </si>
+  <si>
+    <t>0E9D9A52</t>
+  </si>
+  <si>
+    <t>N521D5060011</t>
+  </si>
+  <si>
+    <t>BC590752</t>
+  </si>
+  <si>
+    <t>N521D5060007</t>
+  </si>
+  <si>
+    <t>FECB7890</t>
+  </si>
+  <si>
+    <t>N521D5060010</t>
+  </si>
+  <si>
+    <t>1AF41C46</t>
+  </si>
+  <si>
+    <t>N521D5060014</t>
+  </si>
+  <si>
+    <t>FB2B1B1E</t>
+  </si>
+  <si>
+    <t>N521D5060017</t>
+  </si>
+  <si>
+    <t>D1CECBAB</t>
+  </si>
+  <si>
+    <t>N521D5060029</t>
+  </si>
+  <si>
+    <t>637F447B</t>
+  </si>
+  <si>
+    <t>EAA2FE84</t>
+  </si>
+  <si>
+    <t>N521D5060021</t>
+  </si>
+  <si>
     <t>Joseph Kucmerowski</t>
   </si>
   <si>
-    <t>Joshua Ladd</t>
-  </si>
-  <si>
-    <t>CB46D992</t>
-  </si>
-  <si>
-    <t>N445D50044</t>
-  </si>
-  <si>
-    <t>Justin Blake</t>
-  </si>
-  <si>
-    <t>Justin Sampel</t>
-  </si>
-  <si>
-    <t>Korey Sugar</t>
-  </si>
-  <si>
-    <t>Maria Raquel Pum</t>
-  </si>
-  <si>
-    <t>11D14592</t>
-  </si>
-  <si>
-    <t>N445D50019</t>
-  </si>
-  <si>
-    <t>Mark Zhukov</t>
-  </si>
-  <si>
-    <t>Michael Maksymciw</t>
-  </si>
-  <si>
-    <t>D4C6CF96</t>
-  </si>
-  <si>
-    <t>N515D5060010</t>
-  </si>
-  <si>
-    <t>Michael Tucciarello</t>
-  </si>
-  <si>
-    <t>F72F821E</t>
-  </si>
-  <si>
-    <t>Oleksandr Pogorilov</t>
-  </si>
-  <si>
-    <t>B455EFD2</t>
-  </si>
-  <si>
-    <t>Rashard Moore</t>
-  </si>
-  <si>
-    <t>Reginald Tucker</t>
-  </si>
-  <si>
-    <t>Roedell Williams,</t>
-  </si>
-  <si>
-    <t>0489D091</t>
-  </si>
-  <si>
-    <t>Saad Shamsaldeen</t>
-  </si>
-  <si>
-    <t>Sayed Hossiny</t>
-  </si>
-  <si>
-    <t>BCAFEC01</t>
-  </si>
-  <si>
-    <t>N521D5060027</t>
-  </si>
-  <si>
-    <t>Shondrell Rutley</t>
-  </si>
-  <si>
-    <t>FA02F7A3</t>
-  </si>
-  <si>
-    <t>Steven Dessie</t>
-  </si>
-  <si>
-    <t>Tj Heinlin</t>
-  </si>
-  <si>
-    <t>Zy'Asia Holmes</t>
-  </si>
-  <si>
-    <t>A46E6932</t>
-  </si>
-  <si>
-    <t>N521D5060009</t>
-  </si>
-  <si>
-    <t>N521D5060032</t>
-  </si>
-  <si>
-    <t>N521D5060020</t>
-  </si>
-  <si>
-    <t>N521D5060015</t>
-  </si>
-  <si>
-    <t>N445D50036</t>
-  </si>
-  <si>
-    <t>N521D5060023</t>
-  </si>
-  <si>
-    <t>N521D5060012</t>
-  </si>
-  <si>
-    <t>EC44ACBC</t>
-  </si>
-  <si>
-    <t>N521D5060026</t>
-  </si>
-  <si>
-    <t>3A5DB840</t>
-  </si>
-  <si>
-    <t>N521D5060006</t>
-  </si>
-  <si>
-    <t>52FBA5FF</t>
-  </si>
-  <si>
-    <t>7A21E43A</t>
-  </si>
-  <si>
-    <t>N521D5060004</t>
-  </si>
-  <si>
-    <t>0E9D9A52</t>
-  </si>
-  <si>
-    <t>N521D5060011</t>
-  </si>
-  <si>
-    <t>BC590752</t>
-  </si>
-  <si>
-    <t>N521D5060007</t>
-  </si>
-  <si>
-    <t>FECB7890</t>
-  </si>
-  <si>
-    <t>N521D5060010</t>
-  </si>
-  <si>
-    <t>1AF41C46</t>
-  </si>
-  <si>
-    <t>N521D5060014</t>
-  </si>
-  <si>
-    <t>FB2B1B1E</t>
-  </si>
-  <si>
-    <t>N521D5060017</t>
-  </si>
-  <si>
-    <t>D1CECBAB</t>
-  </si>
-  <si>
-    <t>N521D5060029</t>
-  </si>
-  <si>
-    <t>637F447B</t>
-  </si>
-  <si>
-    <t>EAA2FE84</t>
-  </si>
-  <si>
-    <t>N521D5060021</t>
-  </si>
-  <si>
     <t>Dan Knights</t>
   </si>
   <si>
-    <t>N521D5060018</t>
+    <t>Tj Heinlein</t>
   </si>
 </sst>
 </file>
@@ -433,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,9 +439,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +764,9 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,484 +798,470 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1219</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
-        <v>1216</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>1218</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4">
         <v>1214</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>1194</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>1207</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>1151</v>
       </c>
       <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4">
         <v>1215</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1175</v>
       </c>
       <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>1186</v>
       </c>
       <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>1103</v>
       </c>
       <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
         <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>1127</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="4">
         <v>1190</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>1166</v>
       </c>
       <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>1161</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="B17">
         <v>1180</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>1162</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>1169</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>1125</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21">
         <v>1047</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>1147</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4">
         <v>1217</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4">
         <v>1088</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>1171</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" s="4">
         <v>1182</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27" s="4">
         <v>1174</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>1132</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>1165</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B30">
         <v>1168</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31">
         <v>1116</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" s="4">
         <v>1134</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" s="4">
         <v>1192</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="B34">
         <v>1159</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B35">
         <v>1185</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36">
-        <v>1219</v>
-      </c>
-      <c r="C36" s="7">
-        <v>70626308</v>
-      </c>
-      <c r="D36" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C48">
-    <sortCondition ref="A1:A48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C47">
+    <sortCondition ref="A1:A47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>